<commit_message>
Updated Client Command Table and Code for display
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\SimplicityStudio\v5_workspace\ecen5823-assignment6-DhruvHMehta\questions\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18778F8C-3CBD-430B-A79C-F2C29E14412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -27,7 +36,7 @@
   <si>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -54,7 +63,7 @@
     </r>
     <r>
       <rPr>
-        <b val="1"/>
+        <b/>
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Calibri"/>
@@ -124,42 +133,10 @@
     <t>sl_bt_evt_scanner_scan_report_id</t>
   </si>
   <si>
-    <t>Received for advertising or scan response packets generated by: sl_bt_scanner_start().
-Is the bd_addr, packet_type and address_type what we expect for our Server? If yes:
-   sl_bt_scanner_stop()
-   sl_bt_connection_open()</t>
-  </si>
-  <si>
     <t>sl_bt_evt_gatt_procedure_completed_id</t>
   </si>
   <si>
     <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve">Do not build your state machine into your  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="15"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>handle_ble_event()</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t xml:space="preserve"> function! Instead build a new state machine for A7. </t>
-    </r>
   </si>
   <si>
     <t>sl_bt_evt_gatt_service_id</t>
@@ -180,25 +157,59 @@
     <t>If an indication or notification has been enabled for a characteristic, this event is triggered whenever an indication or notification is received from the remote GATT server.
 Is the characteristic handle and att_opcode we expect? If yes: 
    sl_bt_gatt_send_characteristic_confirmation()</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_discover_primary_services_by_uuid()</t>
+  </si>
+  <si>
+    <t>displayUpdate()</t>
+  </si>
+  <si>
+    <t>Received for advertising or scan response packets generated by: sl_bt_scanner_start().
+Is the bd_addr, packet_type and address_type what we expect for our Server? 
+If yes:
+   sl_bt_scanner_stop()
+   sl_bt_connection_open()
+If no:
+do nothing</t>
+  </si>
+  <si>
+    <t>Save GATT Service handle and GATT UUID</t>
+  </si>
+  <si>
+    <t>Save GATT Characteristics, properties and UUID</t>
+  </si>
+  <si>
+    <t>Save Connection Handle</t>
+  </si>
+  <si>
+    <t>sl_bt_gatt_send_characteristic_confirmation()</t>
+  </si>
+  <si>
+    <t>sl_bt_scanner_stop()
+sl_bt_connection_open()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sl_bt_gatt_discover_characteristics_by_uuid()
+sl_bt_gatt_set_characteristic_notification()
+</t>
+  </si>
+  <si>
+    <t>Client Discovery State Machine (Extra Credit)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="13"/>
@@ -211,7 +222,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -238,8 +249,40 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="15"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -256,7 +299,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -346,84 +389,117 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+  <cellXfs count="36">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,29 +509,1734 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff2236ff"/>
-      <rgbColor rgb="ff4d8f72"/>
-      <rgbColor rgb="ff4d8f72"/>
-      <rgbColor rgb="ff2e74b5"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF2236FF"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="FF4D8F72"/>
+      <rgbColor rgb="FF2E74B5"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16720</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1579190</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>62736</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Oval 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE2E046B-217F-4378-911B-24CBAD9D8A64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4154380" y="10317480"/>
+          <a:ext cx="1562470" cy="1464816"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Get Services</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1797653</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3360123</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>62736</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Oval 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9066E4F7-2A45-4B28-9D16-A279BE401DF4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9204293" y="10317480"/>
+          <a:ext cx="1562470" cy="1464816"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Get Char</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16720</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34918</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1579190</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>158614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Oval 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C9A4B51-6C98-40F9-A2A3-78744D32A879}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4154380" y="14436718"/>
+          <a:ext cx="1562470" cy="1464816"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Receive Data</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1797653</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34918</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3360123</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>158614</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Oval 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D426B025-40D3-42EA-A4D1-A382DE216800}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9204293" y="14436718"/>
+          <a:ext cx="1562470" cy="1464816"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Send Notif</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1579190</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>888</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1797653</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>888</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B9F087D-8748-4CEA-BFC2-1F2653DA6B0D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="6"/>
+          <a:endCxn id="3" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5716850" y="11049888"/>
+          <a:ext cx="3487443" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2578888</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>62736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2578888</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34918</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F0A40C-8632-40C5-B258-71B622653E2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="4"/>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9985528" y="11782296"/>
+          <a:ext cx="0" cy="2654422"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1579190</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>96766</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1797653</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>96766</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{132F50C9-14A3-4234-8FCD-C941DD032E19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="4" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5716850" y="15169126"/>
+          <a:ext cx="3487443" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>797955</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>62736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>797955</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34918</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A728C193-0610-4F64-BC36-893A9BC92042}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="0"/>
+          <a:endCxn id="2" idx="4"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4935615" y="11782296"/>
+          <a:ext cx="0" cy="2654422"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>58150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>89947</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1716277</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>888</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{837E891E-23E4-4C3C-BD8B-BE14CF7A628F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6024610" y="10803667"/>
+          <a:ext cx="3098307" cy="246221"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>sl_bt_gatt_discover_primary_services_by_uuid()</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2613489</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>30205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2859710</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>34919</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B84F14B-0F08-49DB-A2DA-6DFFC5AA05C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="8799763" y="12970131"/>
+          <a:ext cx="2686954" cy="246221"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>sl_bt_gatt_discover_characteristics_by_uuid</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>246595</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>18184</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1527830</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>96765</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79B986EC-87D7-417F-9D54-8561B5BE693B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6213055" y="14922904"/>
+          <a:ext cx="2721415" cy="246221"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>sl_bt_gatt_set_characteristic_notification()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>245538</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>81796</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>797955</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>158615</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Connector: Curved 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5A7F4A8-2F20-4CAF-8B8C-57EA3670C909}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="4" idx="4"/>
+          <a:endCxn id="4" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000" flipH="1">
+          <a:off x="4034257" y="15000177"/>
+          <a:ext cx="1250299" cy="552417"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector5">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -18284"/>
+            <a:gd name="adj2" fmla="val 182803"/>
+            <a:gd name="adj3" fmla="val 118284"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>899160</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>42741</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1402729</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>121322</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="TextBox 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E0C2F7-0DF0-450F-B7E5-A4002CAC5FAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2781300" y="16120941"/>
+          <a:ext cx="2759089" cy="246221"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>sl_bt_gatt_send_characteristic_confirmation()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>521747</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>11265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>767968</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>53857</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="TextBox 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F94887F0-1963-4CD6-AEED-028AE97DC361}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000">
+          <a:off x="4090662" y="12970130"/>
+          <a:ext cx="1383712" cy="246221"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle>
+          <a:defPPr>
+            <a:defRPr lang="en-US"/>
+          </a:defPPr>
+          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
+            <a:defRPr sz="1800" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>sl_bt_scanner_start()</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -657,7 +2438,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -676,7 +2457,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -706,7 +2487,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -732,7 +2513,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -758,7 +2539,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -784,7 +2565,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -810,7 +2591,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -836,7 +2617,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -862,7 +2643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -888,7 +2669,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -914,7 +2695,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -927,9 +2708,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -946,7 +2733,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -965,7 +2752,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -991,7 +2778,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1017,7 +2804,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1043,7 +2830,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1069,7 +2856,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1095,7 +2882,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1121,7 +2908,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1147,7 +2934,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1173,7 +2960,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1199,7 +2986,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1212,9 +2999,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1228,7 +3021,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1247,7 +3040,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1277,7 +3070,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1303,7 +3096,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1329,7 +3122,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1355,7 +3148,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1381,7 +3174,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1407,7 +3200,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1433,7 +3226,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1459,7 +3252,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1485,7 +3278,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1498,346 +3291,389 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:F32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.3516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.6719" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="21" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="44.8516" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="16.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.55" customHeight="1">
+    <row r="1" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" t="s" s="3">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="5"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
     </row>
-    <row r="2" ht="12.05" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+    <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
-    <row r="3" ht="119.55" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" t="s" s="9">
+    <row r="3" spans="1:6" ht="119.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s" s="9">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s" s="9">
+      <c r="D3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s" s="9">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="5"/>
     </row>
-    <row r="4" ht="12.05" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" t="s" s="6">
+    <row r="4" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s" s="9">
+      <c r="C4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s" s="9">
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s" s="9">
+      <c r="E4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s" s="9">
+      <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" ht="13.75" customHeight="1">
-      <c r="A5" t="s" s="10">
+    <row r="5" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
     </row>
-    <row r="6" ht="26.75" customHeight="1">
-      <c r="A6" s="11"/>
-      <c r="B6" t="s" s="11">
+    <row r="6" spans="1:6" ht="26.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-      <c r="E6" t="s" s="14">
+      <c r="C6" s="9"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s" s="15">
+      <c r="F6" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="16"/>
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="16"/>
-      <c r="E7" t="s" s="17">
+      <c r="E7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="12"/>
     </row>
-    <row r="8" ht="13.75" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="16"/>
+    <row r="8" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="16"/>
-      <c r="E8" t="s" s="17">
+      <c r="E8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="15"/>
     </row>
-    <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="16"/>
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="16"/>
-      <c r="E9" t="s" s="17">
+      <c r="E9" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="16"/>
     </row>
-    <row r="10" ht="26.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="16"/>
+    <row r="10" spans="1:6" ht="26.7" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="16"/>
-      <c r="E10" t="s" s="17">
+      <c r="E10" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F10" t="s" s="15">
+      <c r="F10" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" s="7"/>
-      <c r="B12" t="s" s="20">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" t="s" s="20">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="16"/>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" s="7"/>
-      <c r="B16" t="s" s="20">
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" t="s" s="21">
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="19"/>
     </row>
-    <row r="17" ht="13.55" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
     </row>
-    <row r="18" ht="13.55" customHeight="1">
-      <c r="A18" t="s" s="10">
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
     </row>
-    <row r="19" ht="78.75" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" t="s" s="20">
+    <row r="19" spans="1:6" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" t="s" s="21">
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="20" ht="13.55" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="19"/>
+    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
     </row>
-    <row r="21" ht="39.75" customHeight="1">
-      <c r="A21" s="7"/>
-      <c r="B21" t="s" s="20">
-        <v>26</v>
-      </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" t="s" s="21">
+    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F21" t="s" s="23">
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="21" t="s">
         <v>28</v>
       </c>
+      <c r="F23" s="23" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="22" ht="13.55" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="19"/>
-      <c r="F22" s="19"/>
+    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
     </row>
-    <row r="23" ht="13.55" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" t="s" s="20">
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" t="s" s="21">
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F25" s="23" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="24" ht="13.55" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
+    <row r="26" spans="1:6" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
     </row>
-    <row r="25" ht="13.55" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" t="s" s="20">
+    <row r="27" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" t="s" s="21">
+      <c r="C27" s="16"/>
+      <c r="D27" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="19"/>
     </row>
-    <row r="26" ht="13.55" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
+    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
     </row>
-    <row r="27" ht="65.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" t="s" s="20">
-        <v>33</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" t="s" s="21">
-        <v>34</v>
-      </c>
-      <c r="F27" s="19"/>
+    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
     </row>
-    <row r="28" ht="13.55" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-    </row>
-    <row r="29" ht="13.55" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
+    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B32:F32"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added display prints for client, updated command table and bubble diagram and readme.MD
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\SimplicityStudio\v5_workspace\ecen5823-assignment6-DhruvHMehta\questions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\SimplicityStudio\v5_workspace\ecen5823-assignment7-DhruvHMehta\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18778F8C-3CBD-430B-A79C-F2C29E14412E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42EA6B3-0C7E-4CA5-BC4F-A706610CF618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="47">
   <si>
     <t>Client Command Table for A7</t>
   </si>
@@ -200,12 +200,21 @@
   <si>
     <t>Client Discovery State Machine (Extra Credit)</t>
   </si>
+  <si>
+    <t>Discovering</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t>Handling Indications</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -282,6 +291,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -408,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -500,6 +515,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -738,7 +756,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Get Services</a:t>
+            <a:t>OPEN</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -894,9 +912,17 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Get Char</a:t>
+            <a:rPr lang="en-US" sz="1800" i="1" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CHARACTERISTICS</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1052,7 +1078,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US"/>
-            <a:t>Receive Data</a:t>
+            <a:t>CLOSE</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1208,9 +1234,17 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US"/>
-            <a:t>Send Notif</a:t>
+            <a:rPr lang="en-US" sz="1800" i="1" kern="1200">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>NOTIFY</a:t>
           </a:r>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1444,14 +1478,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>58150</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>89947</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>112807</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1716277</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>888</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>164813</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1466,8 +1500,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6024610" y="10803667"/>
-          <a:ext cx="3098307" cy="246221"/>
+          <a:off x="6024610" y="10658887"/>
+          <a:ext cx="3098307" cy="387286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1574,6 +1608,19 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>if(connection_opened)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="0" i="0">
               <a:effectLst/>
@@ -1590,13 +1637,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2613489</xdr:colOff>
+      <xdr:colOff>2573437</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>30205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>2859710</xdr:colOff>
+      <xdr:colOff>2960723</xdr:colOff>
       <xdr:row>58</xdr:row>
       <xdr:rowOff>34919</xdr:rowOff>
     </xdr:to>
@@ -1613,8 +1660,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="8799763" y="12970131"/>
-          <a:ext cx="2686954" cy="246221"/>
+          <a:off x="8830243" y="12899599"/>
+          <a:ext cx="2686954" cy="387286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1721,6 +1768,19 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>if(gatt_completed)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000" b="0" i="0">
+              <a:effectLst/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
           <a:r>
             <a:rPr lang="en-US" sz="1000" b="0" i="0">
               <a:effectLst/>
@@ -1738,14 +1798,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>246595</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>18184</xdr:rowOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>48664</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1527830</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>96765</xdr:rowOff>
+      <xdr:rowOff>100670</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1760,8 +1820,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6213055" y="14922904"/>
-          <a:ext cx="2721415" cy="246221"/>
+          <a:off x="6213055" y="14785744"/>
+          <a:ext cx="2721415" cy="387286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1868,6 +1928,19 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>if(gatt_completed)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
           <a:r>
             <a:rPr lang="en-US" sz="1000">
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -1942,152 +2015,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>899160</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>42741</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1402729</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>121322</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="TextBox 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42E0C2F7-0DF0-450F-B7E5-A4002CAC5FAE}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2781300" y="16120941"/>
-          <a:ext cx="2759089" cy="246221"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr wrap="square" rtlCol="0">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle>
-          <a:defPPr>
-            <a:defRPr lang="en-US"/>
-          </a:defPPr>
-          <a:lvl1pPr marL="0" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" algn="l" defTabSz="914400" rtl="0" eaLnBrk="1" latinLnBrk="0" hangingPunct="1">
-            <a:defRPr sz="1800" kern="1200">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1000">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>sl_bt_gatt_send_characteristic_confirmation()</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>521747</xdr:colOff>
       <xdr:row>46</xdr:row>
@@ -2230,6 +2157,67 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1348740</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>16720</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>888</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C96D640-2F18-4E23-9A35-B336AC49B21E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3230880" y="10447020"/>
+          <a:ext cx="923500" cy="602868"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="none"/>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3315,8 +3303,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:F32"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3398,7 +3386,9 @@
       <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="D6" s="16"/>
       <c r="E6" s="11" t="s">
         <v>12</v>
@@ -3462,7 +3452,9 @@
       <c r="B12" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="16"/>
+      <c r="C12" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="D12" s="25" t="s">
         <v>33</v>
       </c>
@@ -3486,8 +3478,12 @@
       <c r="B14" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>33</v>
+      </c>
       <c r="E14" s="29" t="s">
         <v>17</v>
       </c>
@@ -3538,7 +3534,9 @@
       <c r="B19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="16"/>
+      <c r="C19" s="36" t="s">
+        <v>44</v>
+      </c>
       <c r="D19" s="16"/>
       <c r="E19" s="26" t="s">
         <v>41</v>
@@ -3628,7 +3626,9 @@
       <c r="B27" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="D27" s="25" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Updated Client Command table and bubble diagram
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhruv\SimplicityStudio\v5_workspace\ecen5823-assignment7-DhruvHMehta\questions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42EA6B3-0C7E-4CA5-BC4F-A706610CF618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F3B3AE-ACE5-403A-9B32-2B777B73FACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -207,7 +207,8 @@
     <t>Connected</t>
   </si>
   <si>
-    <t>Handling Indications</t>
+    <t>Handling Indications
+Temp=TemperatureValue</t>
   </si>
 </sst>
 </file>
@@ -504,6 +505,9 @@
     <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -515,9 +519,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2016,13 +2017,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>521747</xdr:colOff>
+      <xdr:colOff>451215</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>11265</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>767968</xdr:colOff>
+      <xdr:colOff>838501</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>53857</xdr:rowOff>
     </xdr:to>
@@ -2039,8 +2040,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000">
-          <a:off x="4090662" y="12970130"/>
-          <a:ext cx="1383712" cy="246221"/>
+          <a:off x="4077962" y="12970718"/>
+          <a:ext cx="1397258" cy="387286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2147,6 +2148,19 @@
           </a:lvl9pPr>
         </a:lstStyle>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>if(connection_closed)</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1000">
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+          </a:br>
           <a:r>
             <a:rPr lang="en-US" sz="1000">
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -3303,8 +3317,8 @@
   </sheetPr>
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B37" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3321,13 +3335,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
@@ -3534,7 +3548,7 @@
       <c r="B19" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="36" t="s">
+      <c r="C19" s="32" t="s">
         <v>44</v>
       </c>
       <c r="D19" s="16"/>
@@ -3656,13 +3670,13 @@
       <c r="F29" s="16"/>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
-      <c r="F32" s="35"/>
+      <c r="C32" s="36"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>